<commit_message>
added weigh1_numbers 2 to meta data
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
   <si>
     <t>nspp</t>
   </si>
@@ -364,13 +364,19 @@
   </si>
   <si>
     <t>NOTE: Most objects are ordered by species code if not specified</t>
+  </si>
+  <si>
+    <t>weight1_Numbers2</t>
+  </si>
+  <si>
+    <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +507,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -847,9 +860,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1174,7 +1188,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="G14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,6 +1475,12 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">

</xml_diff>

<commit_message>
Added ability to estimate srv sigma and changed minage
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="133">
   <si>
     <t>nspp</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Start year of the hindcast</t>
   </si>
   <si>
-    <t>Number of ages of each species included in the hindcast</t>
-  </si>
-  <si>
     <t>Number of lengths of each species included in the hindcast</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic</t>
   </si>
   <si>
-    <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2. Not used otherwise</t>
-  </si>
-  <si>
     <t>Units used for survey: 1 = kg; 2 = numbers</t>
   </si>
   <si>
@@ -370,13 +364,67 @@
   </si>
   <si>
     <t>Minimum age of each species included in the hindcast</t>
+  </si>
+  <si>
+    <t>weight1_Numbers2</t>
+  </si>
+  <si>
+    <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
+  </si>
+  <si>
+    <t>Number of ages of each species included in the hindcast. Includes age 0 if minage = 0</t>
+  </si>
+  <si>
+    <t>Number of ages (starting from minage) to estimate non-parametric selectivity for Selectivity = 2. Not used otherwise</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_catch</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_index</t>
+  </si>
+  <si>
+    <t>Should CEATTLE estimate the variance associated with the catch time series (yes = 1; no = 0). If 0, uses the CV from fsh_biom.</t>
+  </si>
+  <si>
+    <t>Should CEATTLE estimate the variance associated with the survey index time series (yes = 1; no = 0). If 0, uses the CV from srv_biom.</t>
+  </si>
+  <si>
+    <t>Sigma_catch_prior</t>
+  </si>
+  <si>
+    <t>Prior for sigma_catch to be used if Estimate_sigma_catch = 1</t>
+  </si>
+  <si>
+    <t>Sigma_index_prior</t>
+  </si>
+  <si>
+    <t>Prior for sigma_catch to be used if Estimate_sigma_index = 1</t>
+  </si>
+  <si>
+    <t>sigma_rec_prior</t>
+  </si>
+  <si>
+    <t>Prior to be used for estimating the standard deviation around recruitment deviates. Is the starting value if random_rec = TRUE when using fit_mod.</t>
+  </si>
+  <si>
+    <t>projyr</t>
+  </si>
+  <si>
+    <t>End year of the forecast</t>
+  </si>
+  <si>
+    <t>proj_F</t>
+  </si>
+  <si>
+    <t>Projected F rate for forecast of each fishery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +555,19 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,9 +914,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1177,18 +1242,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,713 +1264,777 @@
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="B47" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" s="2" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added analytical q for surveys and analytical sigma
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="127">
   <si>
     <t>nspp</t>
   </si>
@@ -336,9 +336,6 @@
     <t>Age transition matrix (e.g. Age Length Key or ALK) index to use for derived quantitied</t>
   </si>
   <si>
-    <t>Estimate catchability? (0 = no; 1 = yes)</t>
-  </si>
-  <si>
     <t>Starting value or fixed value for catchability</t>
   </si>
   <si>
@@ -370,6 +367,39 @@
   </si>
   <si>
     <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
+  </si>
+  <si>
+    <t>Estimate catchability? (0 = no; 1 = yes, 2 = analytical from Ludwig and Walters 1994)</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_index</t>
+  </si>
+  <si>
+    <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+  </si>
+  <si>
+    <t>Sigma_index_prior</t>
+  </si>
+  <si>
+    <t>Starting value to be used if Estimate_sigma_index = 1</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_catch</t>
+  </si>
+  <si>
+    <t>Estimate fishery variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+  </si>
+  <si>
+    <t>Sigma_catch_prior</t>
+  </si>
+  <si>
+    <t>Starting value to be used if Estimate_sigma_catch = 1</t>
+  </si>
+  <si>
+    <t>NOTE: Lengths are index 1 through nlenths</t>
+  </si>
+  <si>
+    <t>NOTE: Columns for ages are index by 1 trhough nages</t>
   </si>
 </sst>
 </file>
@@ -860,10 +890,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1188,7 +1226,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="F14:G14"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,10 +1251,10 @@
         <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>40</v>
@@ -1276,10 +1314,10 @@
         <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,10 +1334,10 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1439,7 +1477,7 @@
         <v>94</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1455,11 +1493,11 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1475,11 +1513,11 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" t="s">
         <v>115</v>
-      </c>
-      <c r="G14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1495,6 +1533,12 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
+      <c r="F15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1509,11 +1553,14 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1526,8 +1573,14 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1540,8 +1593,14 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1555,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1569,7 +1628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1583,7 +1642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1597,7 +1656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1611,7 +1670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1625,7 +1684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1638,8 +1697,11 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1652,8 +1714,11 @@
       <c r="D26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1666,8 +1731,11 @@
       <c r="D27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1681,7 +1749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1689,13 +1757,13 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1709,7 +1777,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1723,7 +1791,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
added tv q and sel to build params and map and data
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\Rceattle\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F15347-0179-E14B-9092-1C6EA2FC6A68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="139">
   <si>
     <t>nspp</t>
   </si>
@@ -400,13 +401,49 @@
   </si>
   <si>
     <t>NOTE: Columns for ages are index by 1 trhough nages</t>
+  </si>
+  <si>
+    <t>Time_varying_sel</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect.</t>
+  </si>
+  <si>
+    <t>Sel_sd_prior</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying selectivity if set to 1</t>
+  </si>
+  <si>
+    <t>Time_varying_q</t>
+  </si>
+  <si>
+    <t>Q_sd_prior</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying q if set to 1</t>
+  </si>
+  <si>
+    <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect.</t>
+  </si>
+  <si>
+    <t>Selectivity_index</t>
+  </si>
+  <si>
+    <t>index to use if selectivitys of different surveys are to be the same</t>
+  </si>
+  <si>
+    <t>Q_index</t>
+  </si>
+  <si>
+    <t>index to use if catchability coefficients are to be set the same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1222,22 +1259,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1260,7 +1297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1280,7 +1317,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1300,7 +1337,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1340,7 +1377,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1360,7 +1397,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1380,7 +1417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1400,7 +1437,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1420,7 +1457,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1440,7 +1477,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1460,7 +1497,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1480,7 +1517,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1500,7 +1537,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1520,7 +1557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1540,7 +1577,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1560,7 +1597,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1580,7 +1617,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1600,7 +1637,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1613,8 +1650,14 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1627,8 +1670,14 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1641,8 +1690,14 @@
       <c r="D21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1655,8 +1710,14 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1669,8 +1730,14 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1683,8 +1750,14 @@
       <c r="D24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1701,7 +1774,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1718,7 +1791,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1735,7 +1808,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1749,7 +1822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1763,7 +1836,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1777,7 +1850,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1791,7 +1864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1805,7 +1878,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1819,7 +1892,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1833,7 +1906,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1847,7 +1920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1861,7 +1934,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1875,7 +1948,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1889,7 +1962,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1903,7 +1976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1917,7 +1990,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1931,7 +2004,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1945,7 +2018,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1959,7 +2032,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
updated names of sigma index
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F15347-0179-E14B-9092-1C6EA2FC6A68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3E6C21-7787-2F40-8A10-10FEFA542231}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,15 +373,9 @@
     <t>Estimate catchability? (0 = no; 1 = yes, 2 = analytical from Ludwig and Walters 1994)</t>
   </si>
   <si>
-    <t>Estimate_sigma_index</t>
-  </si>
-  <si>
     <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
   </si>
   <si>
-    <t>Sigma_index_prior</t>
-  </si>
-  <si>
     <t>Starting value to be used if Estimate_sigma_index = 1</t>
   </si>
   <si>
@@ -400,9 +394,6 @@
     <t>NOTE: Lengths are index 1 through nlenths</t>
   </si>
   <si>
-    <t>NOTE: Columns for ages are index by 1 trhough nages</t>
-  </si>
-  <si>
     <t>Time_varying_sel</t>
   </si>
   <si>
@@ -437,6 +428,15 @@
   </si>
   <si>
     <t>index to use if catchability coefficients are to be set the same</t>
+  </si>
+  <si>
+    <t>Sigma_survey_prior</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_survey</t>
+  </si>
+  <si>
+    <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1571,10 +1571,10 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" t="s">
         <v>117</v>
-      </c>
-      <c r="G15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1591,10 +1591,10 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="G16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1611,10 +1611,10 @@
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1631,10 +1631,10 @@
         <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1651,10 +1651,10 @@
         <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1671,10 +1671,10 @@
         <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1691,10 +1691,10 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G21" t="s">
         <v>131</v>
-      </c>
-      <c r="G21" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1711,10 +1711,10 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1731,10 +1731,10 @@
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1751,10 +1751,10 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1770,9 +1770,6 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
@@ -1787,9 +1784,6 @@
       <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="F26" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
@@ -1804,9 +1798,6 @@
       <c r="D27" t="s">
         <v>68</v>
       </c>
-      <c r="F27" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
@@ -1835,6 +1826,9 @@
       <c r="D29" t="s">
         <v>68</v>
       </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
@@ -1849,6 +1843,9 @@
       <c r="D30" t="s">
         <v>68</v>
       </c>
+      <c r="F30" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
@@ -1862,6 +1859,9 @@
       </c>
       <c r="D31" t="s">
         <v>68</v>
+      </c>
+      <c r="F31" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7">

</xml_diff>

<commit_message>
updated parameters and time varying selectivity and catachbility in cpp, need to change map function to deal with blocks and such
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\Rceattle\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3E6C21-7787-2F40-8A10-10FEFA542231}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
   <si>
     <t>nspp</t>
   </si>
@@ -397,9 +396,6 @@
     <t>Time_varying_sel</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect.</t>
-  </si>
-  <si>
     <t>Sel_sd_prior</t>
   </si>
   <si>
@@ -415,9 +411,6 @@
     <t>The sd to use for the random walk of time varying q if set to 1</t>
   </si>
   <si>
-    <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect.</t>
-  </si>
-  <si>
     <t>Selectivity_index</t>
   </si>
   <si>
@@ -437,13 +430,19 @@
   </si>
   <si>
     <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
+  </si>
+  <si>
+    <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penalty</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1259,22 +1258,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1317,7 +1316,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1397,7 +1396,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1417,7 +1416,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1457,7 +1456,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1477,7 +1476,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1537,7 +1536,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1571,13 +1570,13 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1591,13 +1590,13 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1654,10 +1653,10 @@
         <v>124</v>
       </c>
       <c r="G19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1671,13 +1670,13 @@
         <v>18</v>
       </c>
       <c r="F20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" t="s">
         <v>126</v>
       </c>
-      <c r="G20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1691,13 +1690,13 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1711,13 +1710,13 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" t="s">
         <v>129</v>
       </c>
-      <c r="G22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1731,13 +1730,13 @@
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1751,13 +1750,13 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1861,10 +1860,10 @@
         <v>68</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1906,7 +1905,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1976,7 +1975,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2004,7 +2003,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2032,7 +2031,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Added polygon plots for survey and age comps
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
   <si>
     <t>nspp</t>
   </si>
@@ -372,15 +372,9 @@
     <t>Estimate catchability? (0 = no; 1 = yes, 2 = analytical from Ludwig and Walters 1994)</t>
   </si>
   <si>
-    <t>Estimate_sigma_index</t>
-  </si>
-  <si>
     <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
   </si>
   <si>
-    <t>Sigma_index_prior</t>
-  </si>
-  <si>
     <t>Starting value to be used if Estimate_sigma_index = 1</t>
   </si>
   <si>
@@ -399,7 +393,49 @@
     <t>NOTE: Lengths are index 1 through nlenths</t>
   </si>
   <si>
-    <t>NOTE: Columns for ages are index by 1 trhough nages</t>
+    <t>Time_varying_sel</t>
+  </si>
+  <si>
+    <t>Sel_sd_prior</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying selectivity if set to 1</t>
+  </si>
+  <si>
+    <t>Time_varying_q</t>
+  </si>
+  <si>
+    <t>Q_sd_prior</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying q if set to 1</t>
+  </si>
+  <si>
+    <t>Selectivity_index</t>
+  </si>
+  <si>
+    <t>index to use if selectivitys of different surveys are to be the same</t>
+  </si>
+  <si>
+    <t>Q_index</t>
+  </si>
+  <si>
+    <t>index to use if catchability coefficients are to be set the same</t>
+  </si>
+  <si>
+    <t>Sigma_survey_prior</t>
+  </si>
+  <si>
+    <t>Estimate_sigma_survey</t>
+  </si>
+  <si>
+    <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
+  </si>
+  <si>
+    <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penalty</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality</t>
   </si>
 </sst>
 </file>
@@ -1225,14 +1261,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1534,10 +1570,10 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" t="s">
         <v>117</v>
-      </c>
-      <c r="G15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1554,10 +1590,10 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,10 +1610,10 @@
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1594,10 +1630,10 @@
         <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,6 +1649,12 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1627,6 +1669,12 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
+      <c r="F20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1641,6 +1689,12 @@
       <c r="D21" t="s">
         <v>19</v>
       </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1655,6 +1709,12 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1669,6 +1729,12 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1683,6 +1749,12 @@
       <c r="D24" t="s">
         <v>22</v>
       </c>
+      <c r="F24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1697,9 +1769,6 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1714,9 +1783,6 @@
       <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="F26" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1731,9 +1797,6 @@
       <c r="D27" t="s">
         <v>68</v>
       </c>
-      <c r="F27" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1762,6 +1825,9 @@
       <c r="D29" t="s">
         <v>68</v>
       </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1776,6 +1842,9 @@
       <c r="D30" t="s">
         <v>68</v>
       </c>
+      <c r="F30" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1789,6 +1858,9 @@
       </c>
       <c r="D31" t="s">
         <v>68</v>
+      </c>
+      <c r="F31" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleans data and updated naming
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="139">
   <si>
     <t>nspp</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Nselages</t>
   </si>
   <si>
-    <t>Catch_units</t>
-  </si>
-  <si>
     <t>Weight_index</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2. Not used otherwise</t>
   </si>
   <si>
-    <t>Units used for survey: 1 = kg; 2 = numbers</t>
-  </si>
-  <si>
     <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
   </si>
   <si>
@@ -436,6 +430,12 @@
   </si>
   <si>
     <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality</t>
+  </si>
+  <si>
+    <t>Fit_0no_1yes</t>
+  </si>
+  <si>
+    <t>Index of wether data should be included in the likelihood and associated parameters estimated.</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,10 +1287,10 @@
         <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>40</v>
@@ -1313,7 +1313,7 @@
         <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1350,10 +1350,10 @@
         <v>60</v>
       </c>
       <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
         <v>109</v>
-      </c>
-      <c r="G4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,10 +1370,10 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
         <v>110</v>
-      </c>
-      <c r="G5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
         <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1410,10 +1410,10 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,16 +1424,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,10 +1450,10 @@
         <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1469,11 +1469,11 @@
       <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="F10" t="s">
-        <v>92</v>
+      <c r="F10" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,10 +1490,10 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1510,10 +1510,10 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1529,11 +1529,11 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>95</v>
+      <c r="F13" t="s">
+        <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1549,11 +1549,11 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>114</v>
+      <c r="F14" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1570,10 +1570,10 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,10 +1590,10 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1610,10 +1610,10 @@
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1630,10 +1630,10 @@
         <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1650,10 +1650,10 @@
         <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1670,10 +1670,10 @@
         <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,10 +1690,10 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,10 +1710,10 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1730,10 +1730,10 @@
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1750,10 +1750,10 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
         <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
         <v>68</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>68</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added ssb bits following dorn
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
   <si>
     <t>nspp</t>
   </si>
@@ -436,6 +436,48 @@
   </si>
   <si>
     <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality</t>
+  </si>
+  <si>
+    <t>projyr</t>
+  </si>
+  <si>
+    <t>End year of the forecast</t>
+  </si>
+  <si>
+    <t>nsex</t>
+  </si>
+  <si>
+    <t>spawn_month</t>
+  </si>
+  <si>
+    <t>Spawning month of the population to adjust the numbers spawning</t>
+  </si>
+  <si>
+    <t>R_sexr</t>
+  </si>
+  <si>
+    <t>Percent of recruitment that is female (ignored if nsex = 1)</t>
+  </si>
+  <si>
+    <t>Number of sexes to model in the population (1 = combined/1sex, 2 = models both female/male)</t>
+  </si>
+  <si>
+    <t>minage</t>
+  </si>
+  <si>
+    <t>Minimum age for each population (i.e.does recruitment correspond to age 0, 1, 2?)</t>
+  </si>
+  <si>
+    <t>ssb_wt_index</t>
+  </si>
+  <si>
+    <t>Weight-at-age (wt) index to use for calculation of each species spawning biomass</t>
+  </si>
+  <si>
+    <t>sigma_rec_prior</t>
+  </si>
+  <si>
+    <t>Standard deviation to use for recruitment</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1403,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -1381,10 +1423,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
         <v>60</v>
@@ -1401,10 +1443,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
         <v>60</v>
@@ -1421,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
@@ -1441,10 +1483,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
@@ -1461,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
         <v>60</v>
@@ -1481,13 +1523,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
         <v>93</v>
@@ -1501,13 +1543,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
         <v>94</v>
@@ -1521,13 +1563,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>95</v>
@@ -1541,13 +1583,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>114</v>
@@ -1561,13 +1603,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>135</v>
@@ -1581,13 +1623,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>134</v>
@@ -1601,13 +1643,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>119</v>
@@ -1618,16 +1660,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>121</v>
@@ -1638,16 +1680,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
         <v>124</v>
@@ -1658,16 +1700,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
         <v>125</v>
@@ -1678,16 +1720,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>127</v>
@@ -1698,16 +1740,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
         <v>128</v>
@@ -1718,16 +1760,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
         <v>130</v>
@@ -1738,16 +1780,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
         <v>132</v>
@@ -1758,72 +1800,72 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F29" t="s">
         <v>113</v>
@@ -1831,16 +1873,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
         <v>123</v>
@@ -1848,16 +1890,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="F31" t="s">
         <v>136</v>
@@ -1865,41 +1907,41 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
         <v>68</v>
@@ -1907,13 +1949,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
         <v>68</v>
@@ -1921,13 +1963,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
         <v>68</v>
@@ -1935,13 +1977,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
         <v>68</v>
@@ -1949,99 +1991,197 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B51" t="s">
         <v>81</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
         <v>85</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D51" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started update on sex specific model
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="155">
   <si>
     <t>nspp</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Standard deviation to use for recruitment</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>sex codes: 0=combined; 1=use female only; 2=use male only</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1310,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,10 +1458,10 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,10 +1478,10 @@
         <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1492,10 +1498,10 @@
         <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1512,10 +1518,10 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1532,10 +1538,10 @@
         <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,10 +1558,10 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1571,11 +1577,11 @@
       <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>95</v>
+      <c r="F13" t="s">
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1591,11 +1597,11 @@
       <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>114</v>
+      <c r="F14" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1611,11 +1617,11 @@
       <c r="D15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>135</v>
+      <c r="F15" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="G15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,11 +1637,11 @@
       <c r="D16" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>134</v>
+      <c r="F16" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1651,11 +1657,11 @@
       <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>119</v>
+      <c r="F17" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1672,10 +1678,10 @@
         <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1691,11 +1697,11 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" t="s">
-        <v>124</v>
+      <c r="F19" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="G19" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,10 +1718,10 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,10 +1738,10 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,10 +1758,10 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1772,10 +1778,10 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,10 +1798,10 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1810,6 +1816,12 @@
       </c>
       <c r="D25" t="s">
         <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated non-parametric selectivity penalties
Updated choice of non-parametric selectivity penalties. They are now set using Time_varying_sel and Sel_sd_prior. At some point I should change the naming convention to Sel_setting_1, Sel_setting_2 or similar
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\Rceattle\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0BF229-F42D-1249-8354-90EAE7EBF434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="161">
   <si>
     <t>nspp</t>
   </si>
@@ -201,9 +202,6 @@
     <t>Weight-at-age (wt) to use for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). Can have multiple weight-at-age data-sets for each species, but must be full for all years of the hindcast.</t>
   </si>
   <si>
-    <t>control</t>
-  </si>
-  <si>
     <t>Sheet location</t>
   </si>
   <si>
@@ -225,9 +223,6 @@
     <t>data_list Object name</t>
   </si>
   <si>
-    <t>bioenergetics_control</t>
-  </si>
-  <si>
     <t>This scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Page</t>
   </si>
   <si>
@@ -252,9 +247,6 @@
     <t>Annual relative foraging rate by age</t>
   </si>
   <si>
-    <t>Temp_data</t>
-  </si>
-  <si>
     <t>UobsAge</t>
   </si>
   <si>
@@ -279,12 +271,6 @@
     <t>Stomach proportion by weight for each predator, prey, predator length prey length combination. Can also be year specific by including the column, "Year"</t>
   </si>
   <si>
-    <t>Survey_name</t>
-  </si>
-  <si>
-    <t>Survey_code</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -306,15 +292,6 @@
     <t>Estimate_q</t>
   </si>
   <si>
-    <t>log_q_start</t>
-  </si>
-  <si>
-    <t>Name of survey</t>
-  </si>
-  <si>
-    <t>Index of survey ACROSS species</t>
-  </si>
-  <si>
     <t>Species number</t>
   </si>
   <si>
@@ -348,18 +325,6 @@
     <t>Column names</t>
   </si>
   <si>
-    <t>Fishery_name</t>
-  </si>
-  <si>
-    <t>Fishery_code</t>
-  </si>
-  <si>
-    <t>Name of fishery</t>
-  </si>
-  <si>
-    <t>Index of fishery ACROSS species</t>
-  </si>
-  <si>
     <t>NOTE: Most objects are ordered by species code if not specified</t>
   </si>
   <si>
@@ -378,15 +343,9 @@
     <t>Starting value to be used if Estimate_sigma_index = 1</t>
   </si>
   <si>
-    <t>Estimate_sigma_catch</t>
-  </si>
-  <si>
     <t>Estimate fishery variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
   </si>
   <si>
-    <t>Sigma_catch_prior</t>
-  </si>
-  <si>
     <t>Starting value to be used if Estimate_sigma_catch = 1</t>
   </si>
   <si>
@@ -399,9 +358,6 @@
     <t>Sel_sd_prior</t>
   </si>
   <si>
-    <t>The sd to use for the random walk of time varying selectivity if set to 1</t>
-  </si>
-  <si>
     <t>Time_varying_q</t>
   </si>
   <si>
@@ -423,21 +379,12 @@
     <t>index to use if catchability coefficients are to be set the same</t>
   </si>
   <si>
-    <t>Sigma_survey_prior</t>
-  </si>
-  <si>
-    <t>Estimate_sigma_survey</t>
-  </si>
-  <si>
     <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
   </si>
   <si>
     <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penalty</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality</t>
-  </si>
-  <si>
     <t>projyr</t>
   </si>
   <si>
@@ -483,13 +430,85 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>sex codes: 0=combined; 1=use female only; 2=use male only</t>
+    <t>fleet_control</t>
+  </si>
+  <si>
+    <t>Fleet_name</t>
+  </si>
+  <si>
+    <t>Fleet_code</t>
+  </si>
+  <si>
+    <t>Name of survey or fishery</t>
+  </si>
+  <si>
+    <t>Index of survey/fishery ACROSS species</t>
+  </si>
+  <si>
+    <t>Fleet_type</t>
+  </si>
+  <si>
+    <t>0 = Do not estimate; 1 = Fishery; 2 = Survey</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying selectivity if set to 1. If selectivity is set to type = 2 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>Age_first_selected</t>
+  </si>
+  <si>
+    <t>Age at which selectivity is non-zero</t>
+  </si>
+  <si>
+    <t>Acuumulation_age_lower</t>
+  </si>
+  <si>
+    <t>Ages below this will be grouped to this age for composition data. For example, if set to 2, comp data for age 2 will include 1 and 2 year olds.</t>
+  </si>
+  <si>
+    <t>Acuumulation_age_upper</t>
+  </si>
+  <si>
+    <t>Ages above this will be grouped to this age for composition data. For example, if set to 9 for a species with 10 ages, comp data for age 9 will include 9 and 10 year olds.</t>
+  </si>
+  <si>
+    <t>Log_q_prior</t>
+  </si>
+  <si>
+    <t>Survey_sd_prior</t>
+  </si>
+  <si>
+    <t>Estimate_survey_sd</t>
+  </si>
+  <si>
+    <t>Estimate_catch_sd</t>
+  </si>
+  <si>
+    <t>Catch_sd_prior</t>
+  </si>
+  <si>
+    <t>Comp_weights</t>
+  </si>
+  <si>
+    <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
+  </si>
+  <si>
+    <t>proj_F_prop</t>
+  </si>
+  <si>
+    <t>The proportion of future fishing mortality assigned to this fleet</t>
+  </si>
+  <si>
+    <t>sex codes: 0=combined; 1=use female only; 2=use male only; 3 = joint female and male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1306,45 +1325,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1355,16 +1374,16 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1375,16 +1394,16 @@
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1395,96 +1414,96 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1495,36 +1514,36 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1535,16 +1554,16 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1555,36 +1574,36 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
         <v>149</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>150</v>
       </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1592,39 +1611,39 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
         <v>103</v>
       </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>114</v>
+        <v>136</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1635,16 +1654,16 @@
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1655,16 +1674,16 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
       </c>
       <c r="G17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1675,16 +1694,16 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>119</v>
+        <v>136</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1695,16 +1714,16 @@
         <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1715,16 +1734,16 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="G20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1735,16 +1754,16 @@
         <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>14</v>
       </c>
@@ -1755,16 +1774,16 @@
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>127</v>
+        <v>136</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="G22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>15</v>
       </c>
@@ -1775,16 +1794,16 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" t="s">
-        <v>128</v>
+        <v>136</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>16</v>
       </c>
@@ -1795,16 +1814,16 @@
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="G24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1815,16 +1834,16 @@
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="G25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>18</v>
       </c>
@@ -1835,10 +1854,16 @@
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>19</v>
       </c>
@@ -1849,10 +1874,16 @@
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1863,10 +1894,16 @@
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>21</v>
       </c>
@@ -1874,16 +1911,10 @@
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>22</v>
       </c>
@@ -1891,16 +1922,16 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="G30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1908,16 +1939,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1925,13 +1950,10 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1939,13 +1961,13 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1953,13 +1975,13 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1967,13 +1989,13 @@
         <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>28</v>
       </c>
@@ -1981,13 +2003,11 @@
         <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1995,13 +2015,10 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -2009,13 +2026,10 @@
         <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>31</v>
       </c>
@@ -2023,13 +2037,10 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>32</v>
       </c>
@@ -2037,13 +2048,10 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>33</v>
       </c>
@@ -2051,13 +2059,10 @@
         <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>34</v>
       </c>
@@ -2065,13 +2070,10 @@
         <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>35</v>
       </c>
@@ -2079,13 +2081,10 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>36</v>
       </c>
@@ -2093,13 +2092,10 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>37</v>
       </c>
@@ -2107,13 +2103,10 @@
         <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>38</v>
       </c>
@@ -2121,13 +2114,10 @@
         <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>39</v>
       </c>
@@ -2135,66 +2125,51 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
-      </c>
-      <c r="D47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>85</v>
-      </c>
-      <c r="D51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ceattle to not bug out for 1 species models
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\Rceattle\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0BF229-F42D-1249-8354-90EAE7EBF434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -295,9 +294,6 @@
     <t>Species number</t>
   </si>
   <si>
-    <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic</t>
-  </si>
-  <si>
     <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2. Not used otherwise</t>
   </si>
   <si>
@@ -503,12 +499,15 @@
   </si>
   <si>
     <t>sex codes: 0=combined; 1=use female only; 2=use male only; 3 = joint female and male</t>
+  </si>
+  <si>
+    <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1325,22 +1324,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1354,16 +1353,16 @@
         <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1374,16 +1373,16 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
         <v>136</v>
       </c>
-      <c r="F2" t="s">
-        <v>137</v>
-      </c>
       <c r="G2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1394,16 +1393,16 @@
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1414,27 +1413,27 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
         <v>141</v>
       </c>
-      <c r="G4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
         <v>83</v>
@@ -1443,67 +1442,67 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
         <v>115</v>
       </c>
-      <c r="G6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
         <v>124</v>
       </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F7" t="s">
         <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
         <v>126</v>
       </c>
-      <c r="C8" t="s">
-        <v>127</v>
-      </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1514,36 +1513,36 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1554,16 +1553,16 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G11" t="s">
         <v>145</v>
       </c>
-      <c r="G11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1574,36 +1573,36 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" t="s">
         <v>147</v>
       </c>
-      <c r="G12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
         <v>131</v>
       </c>
-      <c r="C13" t="s">
-        <v>132</v>
-      </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" t="s">
         <v>149</v>
       </c>
-      <c r="G13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1611,39 +1610,39 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
         <v>102</v>
       </c>
-      <c r="G14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
         <v>133</v>
       </c>
-      <c r="C15" t="s">
-        <v>134</v>
-      </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
         <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1654,16 +1653,16 @@
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1674,16 +1673,16 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" t="s">
         <v>117</v>
       </c>
-      <c r="G17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1694,16 +1693,16 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
         <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1714,16 +1713,16 @@
         <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1734,16 +1733,16 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1754,16 +1753,16 @@
         <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
         <v>113</v>
       </c>
-      <c r="G21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -1774,16 +1773,16 @@
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -1794,16 +1793,16 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -1814,16 +1813,16 @@
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1834,16 +1833,16 @@
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
@@ -1854,16 +1853,16 @@
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" t="s">
         <v>156</v>
       </c>
-      <c r="G26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -1874,16 +1873,16 @@
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
         <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1894,16 +1893,16 @@
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" t="s">
         <v>158</v>
       </c>
-      <c r="G28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
@@ -1925,13 +1924,13 @@
         <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1953,7 +1952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1964,10 +1963,10 @@
         <v>65</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1978,10 +1977,10 @@
         <v>73</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1992,10 +1991,10 @@
         <v>67</v>
       </c>
       <c r="F35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
@@ -2003,11 +2002,11 @@
         <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>31</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>32</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>33</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>34</v>
       </c>
@@ -2073,7 +2072,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>35</v>
       </c>
@@ -2084,7 +2083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>36</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>37</v>
       </c>
@@ -2106,7 +2105,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>38</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>39</v>
       </c>
@@ -2128,7 +2127,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>40</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>41</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>42</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Martin's Likes, Analytical q change, Q prior
Added martin's likelihoods to cpp
Updated analytical q to account for time varying sigma as input by user
Changed q selection to have a prior on q
1 = est param, 2 = est param with prior, 3 = analytical, 4 = power function
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -450,9 +450,6 @@
     <t>The sd to use for the random walk of time varying selectivity if set to 1. If selectivity is set to type = 2 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penality. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
-  </si>
-  <si>
     <t>Age_first_selected</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity, or descending logistic. 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1328,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1479,7 @@
         <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1519,7 +1519,7 @@
         <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1556,10 +1556,10 @@
         <v>135</v>
       </c>
       <c r="F11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" t="s">
         <v>144</v>
-      </c>
-      <c r="G11" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,10 +1576,10 @@
         <v>135</v>
       </c>
       <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" t="s">
         <v>146</v>
-      </c>
-      <c r="G12" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,10 +1596,10 @@
         <v>135</v>
       </c>
       <c r="F13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" t="s">
         <v>148</v>
-      </c>
-      <c r="G13" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1716,7 +1716,7 @@
         <v>135</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G19" t="s">
         <v>96</v>
@@ -1776,7 +1776,7 @@
         <v>135</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G22" t="s">
         <v>104</v>
@@ -1796,7 +1796,7 @@
         <v>135</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G23" t="s">
         <v>105</v>
@@ -1816,7 +1816,7 @@
         <v>135</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" t="s">
         <v>106</v>
@@ -1836,7 +1836,7 @@
         <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G25" t="s">
         <v>107</v>
@@ -1856,10 +1856,10 @@
         <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" t="s">
         <v>155</v>
-      </c>
-      <c r="G26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,10 +1896,10 @@
         <v>135</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" t="s">
         <v>157</v>
-      </c>
-      <c r="G28" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
         <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added sex ratio to likelihood, changed propF to sex_ratio
For two sex models, added sex ratio to the model likelihood. The use inputs the mean in the sex_ratio data and the variance in the control. est_sex_ratio = 0, does not estimate; 1 = estimate using annual mean across ages (uses age2 in sex_ratio), 2 = estimate using annual and age specific estimates.
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="160">
   <si>
     <t>nspp</t>
   </si>
@@ -48,30 +48,18 @@
     <t>stom_sample_size</t>
   </si>
   <si>
-    <t>srv_control</t>
-  </si>
-  <si>
     <t>srv_biom</t>
   </si>
   <si>
     <t>srv_emp_sel</t>
   </si>
   <si>
-    <t>srv_comp</t>
-  </si>
-  <si>
-    <t>fsh_control</t>
-  </si>
-  <si>
     <t>fsh_biom</t>
   </si>
   <si>
     <t>fsh_emp_sel</t>
   </si>
   <si>
-    <t>fsh_comp</t>
-  </si>
-  <si>
     <t>age_trans_matrix</t>
   </si>
   <si>
@@ -168,18 +156,9 @@
     <t>Sample size of diet data for each species (used when suitMode &gt; 0)</t>
   </si>
   <si>
-    <t>Survey data specifications</t>
-  </si>
-  <si>
     <t>Empirical selectivity for surveys (leave empty if not used)</t>
   </si>
   <si>
-    <t>Survey age or length composition data</t>
-  </si>
-  <si>
-    <t>Fishery data specifications</t>
-  </si>
-  <si>
     <t>Total catch in weight (kg) or numbers data</t>
   </si>
   <si>
@@ -189,9 +168,6 @@
     <t>Empirical selectivity for fisheries (leave empty if not used)</t>
   </si>
   <si>
-    <t>Fishery age or length composition data</t>
-  </si>
-  <si>
     <t>Age transition matrix (e.g. Age Length Key or ALK) used to convert age to length for length comp data. Can have multiple ALKs for a species specified by ALK_index.</t>
   </si>
   <si>
@@ -502,6 +478,27 @@
   </si>
   <si>
     <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity, or descending logistic. 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>Survey and fishery data specifications</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>Survey/fishery age or length composition data</t>
+  </si>
+  <si>
+    <t>est_propF</t>
+  </si>
+  <si>
+    <t>propF_sigma</t>
+  </si>
+  <si>
+    <t>Is sex ration F/(M+F) to be included in the likelihood (assumed normal); 0 = no, 1 = use annual average across ages (uses 2nd age in propF data), 2 = age, and year specific (TBD)</t>
+  </si>
+  <si>
+    <t>Initial value or fixed value for sd of normal likelihood for sex ration. Not yet able to estimate.</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,25 +1338,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,16 +1367,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,16 +1387,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1410,16 +1407,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,19 +1424,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,19 +1444,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1467,19 +1464,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1487,19 +1484,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1510,16 +1507,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,19 +1524,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,16 +1547,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" t="s">
         <v>135</v>
       </c>
-      <c r="F11" t="s">
-        <v>143</v>
-      </c>
       <c r="G11" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1570,16 +1567,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F12" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G12" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1587,19 +1584,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G13" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1610,16 +1607,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" t="s">
         <v>94</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1627,19 +1624,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1650,16 +1647,16 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1670,16 +1667,16 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1687,19 +1684,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1707,19 +1704,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1727,19 +1724,19 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" t="s">
         <v>111</v>
-      </c>
-      <c r="G20" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,19 +1744,19 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1767,19 +1764,19 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1787,19 +1784,19 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1807,19 +1804,19 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,19 +1824,19 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1847,19 +1844,19 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G26" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1867,19 +1864,19 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1887,19 +1884,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G28" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,10 +1904,10 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,16 +1915,16 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1935,10 +1932,10 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1946,10 +1943,10 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,13 +1954,13 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,13 +1968,13 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,13 +1982,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,10 +1996,10 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F36" s="4"/>
     </row>
@@ -2011,10 +2008,10 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,10 +2019,10 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2033,10 +2030,10 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2044,10 +2041,10 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,10 +2052,10 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2066,10 +2063,10 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,10 +2074,10 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2088,10 +2085,10 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,10 +2096,10 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2110,10 +2107,10 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2121,10 +2118,10 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,10 +2129,10 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,10 +2140,10 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,10 +2151,10 @@
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,10 +2162,10 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allowed multiple environmental indices and environmentally driven q
Allowed for multiple environmental indices by changing BTemp to env_data and inputting as matrix
Bioenegetics is driven by the index selected by Cindex
Added Estimate_q = 5, where catchability ln(q_y) = q_mu + beta * index_y. Where the index is selected by the Time_varying_q column in fleet control
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="162">
   <si>
     <t>nspp</t>
   </si>
@@ -117,12 +117,6 @@
     <t>CK4</t>
   </si>
   <si>
-    <t>Tyrs</t>
-  </si>
-  <si>
-    <t>BTempC</t>
-  </si>
-  <si>
     <t>Pyrs</t>
   </si>
   <si>
@@ -210,12 +204,6 @@
     <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
   </si>
   <si>
-    <t xml:space="preserve">Years of bottom temperature data to incorporate into ft specificed by Ceq. </t>
-  </si>
-  <si>
-    <t>Bottom temperature data to incorporate into ft specificed by Ceq. Will use the mean for missing years.</t>
-  </si>
-  <si>
     <t>Which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979)</t>
   </si>
   <si>
@@ -306,9 +294,6 @@
     <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
   </si>
   <si>
-    <t>Estimate catchability? (0 = no; 1 = yes, 2 = analytical from Ludwig and Walters 1994)</t>
-  </si>
-  <si>
     <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
   </si>
   <si>
@@ -354,9 +339,6 @@
     <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
   </si>
   <si>
-    <t>Wether a time-varying q should be estimated. 0 = no, 1 = random walk from mean selectivity following Dorn 2018, 2 = random effect, 3 = time blocks with no penalty</t>
-  </si>
-  <si>
     <t>projyr</t>
   </si>
   <si>
@@ -444,9 +426,6 @@
     <t>Ages above this will be grouped to this age for composition data. For example, if set to 9 for a species with 10 ages, comp data for age 9 will include 9 and 10 year olds.</t>
   </si>
   <si>
-    <t>Log_q_prior</t>
-  </si>
-  <si>
     <t>Survey_sd_prior</t>
   </si>
   <si>
@@ -477,9 +456,6 @@
     <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity, or descending logistic. 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
-  </si>
-  <si>
     <t>Survey and fishery data specifications</t>
   </si>
   <si>
@@ -499,6 +475,36 @@
   </si>
   <si>
     <t>Initial value or fixed value for sd of normal likelihood for sex ration. Not yet able to estimate.</t>
+  </si>
+  <si>
+    <t>Q_prior</t>
+  </si>
+  <si>
+    <t>Time_varying_q_sd_prior</t>
+  </si>
+  <si>
+    <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity, or descending logistic. 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 2 = random effect, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y</t>
+  </si>
+  <si>
+    <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
+  </si>
+  <si>
+    <t>Cindex</t>
+  </si>
+  <si>
+    <t>Which environmental index in env_data to use to drive bioenergetics</t>
+  </si>
+  <si>
+    <t>env_data</t>
+  </si>
+  <si>
+    <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,25 +1344,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1367,16 +1373,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1387,16 +1393,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1407,16 +1413,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" t="s">
         <v>127</v>
-      </c>
-      <c r="F4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,19 +1430,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,19 +1450,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1464,19 +1470,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1484,19 +1490,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1507,16 +1513,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1524,19 +1530,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,16 +1553,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1567,16 +1573,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1584,19 +1590,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1607,16 +1613,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,19 +1630,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1647,16 +1653,16 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1667,16 +1673,16 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1684,19 +1690,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1704,19 +1710,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1724,19 +1730,19 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,16 +1753,16 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1767,16 +1773,16 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>143</v>
+        <v>121</v>
+      </c>
+      <c r="F22" t="s">
+        <v>153</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1784,19 +1790,19 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>142</v>
+        <v>121</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1807,16 +1813,16 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>144</v>
+        <v>121</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="G24" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,16 +1833,16 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="G25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1847,16 +1853,16 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G26" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1867,16 +1873,16 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" t="s">
-        <v>78</v>
+        <v>121</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1887,16 +1893,16 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>148</v>
+        <v>121</v>
+      </c>
+      <c r="F28" t="s">
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,7 +1913,13 @@
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,13 +1930,13 @@
         <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G30" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1935,7 +1947,7 @@
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1946,7 +1958,7 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,10 +1969,10 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,10 +1983,10 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1982,13 +1994,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1996,33 +2008,33 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="4"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2030,10 +2042,10 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2041,10 +2053,10 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2052,10 +2064,10 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2063,10 +2075,10 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2074,10 +2086,10 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2085,10 +2097,10 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2096,10 +2108,10 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,10 +2119,10 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,10 +2130,10 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2129,10 +2141,10 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" t="s">
         <v>67</v>
-      </c>
-      <c r="C48" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2140,10 +2152,10 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
         <v>68</v>
-      </c>
-      <c r="C49" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2151,10 +2163,10 @@
         <v>42</v>
       </c>
       <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
         <v>69</v>
-      </c>
-      <c r="C50" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2162,10 +2174,10 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
         <v>70</v>
-      </c>
-      <c r="C51" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated meta_names in excel, added optimization control to fit mod
Added optimization control to fit_mod and phaser
F now is zero for non-fisheries. Was previously unused for surveys but set at the initial parameter values that were not estimated. Now set to zero.
Removed the environmental q bit in the cpp file because it was giving the cod model some trouble.
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="156">
   <si>
     <t>nspp</t>
   </si>
@@ -51,15 +51,9 @@
     <t>srv_biom</t>
   </si>
   <si>
-    <t>srv_emp_sel</t>
-  </si>
-  <si>
     <t>fsh_biom</t>
   </si>
   <si>
-    <t>fsh_emp_sel</t>
-  </si>
-  <si>
     <t>age_trans_matrix</t>
   </si>
   <si>
@@ -150,18 +144,12 @@
     <t>Sample size of diet data for each species (used when suitMode &gt; 0)</t>
   </si>
   <si>
-    <t>Empirical selectivity for surveys (leave empty if not used)</t>
-  </si>
-  <si>
     <t>Total catch in weight (kg) or numbers data</t>
   </si>
   <si>
     <t>Survey index in weight (kg) or numbers data</t>
   </si>
   <si>
-    <t>Empirical selectivity for fisheries (leave empty if not used)</t>
-  </si>
-  <si>
     <t>Age transition matrix (e.g. Age Length Key or ALK) used to convert age to length for length comp data. Can have multiple ALKs for a species specified by ALK_index.</t>
   </si>
   <si>
@@ -189,12 +177,6 @@
     <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
   </si>
   <si>
-    <t>data_list Object name</t>
-  </si>
-  <si>
-    <t>This scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Page</t>
-  </si>
-  <si>
     <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
   </si>
   <si>
@@ -207,33 +189,18 @@
     <t>Which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979)</t>
   </si>
   <si>
-    <t>Annual relative foraging rate by age</t>
-  </si>
-  <si>
     <t>UobsAge</t>
   </si>
   <si>
     <t>UobsWtAge</t>
   </si>
   <si>
-    <t>Uobs</t>
-  </si>
-  <si>
-    <t>UobsWt</t>
-  </si>
-  <si>
     <t>Stomach proportion by numbers for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
   </si>
   <si>
     <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
   </si>
   <si>
-    <t>Stomach proportion by numbers for each predator, prey, predator length, prey length combination. Can also be year specific by including the column, "Year"</t>
-  </si>
-  <si>
-    <t>Stomach proportion by weight for each predator, prey, predator length prey length combination. Can also be year specific by including the column, "Year"</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -276,9 +243,6 @@
     <t>Starting value or fixed value for catchability</t>
   </si>
   <si>
-    <t>Percent of foraging days per year for each species</t>
-  </si>
-  <si>
     <t>Blank</t>
   </si>
   <si>
@@ -327,9 +291,6 @@
     <t>Selectivity_index</t>
   </si>
   <si>
-    <t>index to use if selectivitys of different surveys are to be the same</t>
-  </si>
-  <si>
     <t>Q_index</t>
   </si>
   <si>
@@ -459,12 +420,6 @@
     <t>Survey and fishery data specifications</t>
   </si>
   <si>
-    <t>comp</t>
-  </si>
-  <si>
-    <t>Survey/fishery age or length composition data</t>
-  </si>
-  <si>
     <t>est_propF</t>
   </si>
   <si>
@@ -505,6 +460,33 @@
   </si>
   <si>
     <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
+  </si>
+  <si>
+    <t>emp_sel</t>
+  </si>
+  <si>
+    <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
+  </si>
+  <si>
+    <t>comp_data</t>
+  </si>
+  <si>
+    <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
+  </si>
+  <si>
+    <t>Object name</t>
+  </si>
+  <si>
+    <t>index to use if selectivities of different surveys are to be the same</t>
+  </si>
+  <si>
+    <t>Number of foraging days per year for each species</t>
+  </si>
+  <si>
+    <t>This scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
+  </si>
+  <si>
+    <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,25 +1326,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1373,16 +1355,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,16 +1375,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,16 +1395,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1430,19 +1412,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,19 +1432,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,19 +1452,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,19 +1472,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,16 +1495,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,19 +1512,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
         <v>115</v>
-      </c>
-      <c r="D10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1553,16 +1535,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1573,16 +1555,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,19 +1572,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" t="s">
         <v>121</v>
-      </c>
-      <c r="F13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,16 +1595,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1630,19 +1612,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1653,16 +1635,16 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,16 +1655,16 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,19 +1672,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,19 +1692,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1730,19 +1712,19 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1753,16 +1735,16 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,16 +1755,16 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1790,19 +1772,19 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G23" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1810,19 +1792,19 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1830,19 +1812,19 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1850,19 +1832,19 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1870,19 +1852,19 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1890,19 +1872,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,16 +1892,16 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="G29" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1927,16 +1909,16 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G30" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1944,10 +1926,10 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1955,10 +1937,10 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,13 +1948,13 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1980,13 +1962,13 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1994,13 +1976,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,10 +1990,10 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,10 +2001,10 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2031,10 +2013,10 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,10 +2024,10 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2053,10 +2035,10 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2064,10 +2046,10 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2075,10 +2057,10 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2086,10 +2068,10 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,10 +2079,10 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2108,10 +2090,10 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,10 +2101,10 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2130,10 +2112,10 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,43 +2123,10 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>41</v>
-      </c>
-      <c r="B49" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>42</v>
-      </c>
-      <c r="B50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>43</v>
-      </c>
-      <c r="B51" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed ALK to Age_transition where appropriate
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -39,9 +39,6 @@
     <t>pop_wt_index</t>
   </si>
   <si>
-    <t>pop_alk_index</t>
-  </si>
-  <si>
     <t>other_food</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Survey index in weight (kg) or numbers data</t>
   </si>
   <si>
-    <t>Age transition matrix (e.g. Age Length Key or ALK) used to convert age to length for length comp data. Can have multiple ALKs for a species specified by ALK_index.</t>
-  </si>
-  <si>
     <t>Aging error matrices. Can have only one per species.</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>Weight_index</t>
   </si>
   <si>
-    <t>ALK_index</t>
-  </si>
-  <si>
     <t>Estimate_q</t>
   </si>
   <si>
@@ -234,12 +225,6 @@
     <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
   </si>
   <si>
-    <t>Age transition matrix (e.g. Age Length Key or ALK) index to use for derived quantities of the population (used in length-based predation estimation)</t>
-  </si>
-  <si>
-    <t>Age transition matrix (e.g. Age Length Key or ALK) index to use for derived quantitied</t>
-  </si>
-  <si>
     <t>Starting value or fixed value for catchability</t>
   </si>
   <si>
@@ -487,6 +472,21 @@
   </si>
   <si>
     <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
+  </si>
+  <si>
+    <t>pop_age_transition_index</t>
+  </si>
+  <si>
+    <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities of the population to convert age to length (also used in length-based predation estimation)</t>
+  </si>
+  <si>
+    <t>Age_transition_index</t>
+  </si>
+  <si>
+    <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
+  </si>
+  <si>
+    <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. Can have multiple matrices for a species specified by Age_transition_index.</t>
   </si>
 </sst>
 </file>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,25 +1326,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,16 +1355,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1375,16 +1375,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1395,16 +1395,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" t="s">
         <v>108</v>
       </c>
-      <c r="F4" t="s">
-        <v>113</v>
-      </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,19 +1412,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1432,19 +1432,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1452,19 +1452,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,19 +1472,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1495,16 +1495,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1512,19 +1512,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1535,16 +1535,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1555,16 +1555,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1572,19 +1572,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,19 +1592,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1612,19 +1612,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,19 +1632,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1652,19 +1652,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1672,19 +1672,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1692,19 +1692,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,19 +1712,19 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,19 +1732,19 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,19 +1752,19 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1772,19 +1772,19 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,19 +1792,19 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,19 +1812,19 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,19 +1832,19 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1852,19 +1852,19 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1872,19 +1872,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1892,16 +1892,16 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G29" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1909,16 +1909,16 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G30" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1926,10 +1926,10 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1937,10 +1937,10 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,13 +1976,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1990,10 +1990,10 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,10 +2001,10 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2013,10 +2013,10 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2024,10 +2024,10 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2035,10 +2035,10 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2046,10 +2046,10 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2057,10 +2057,10 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2068,10 +2068,10 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,10 +2079,10 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,10 +2090,10 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2101,10 +2101,10 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2112,10 +2112,10 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
         <v>56</v>
-      </c>
-      <c r="C47" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2123,10 +2123,10 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
         <v>57</v>
-      </c>
-      <c r="C48" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed some old files and updated roxygen for data and fixed age_trans name bug from last commit
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="156">
   <si>
     <t>nspp</t>
   </si>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,6 +1897,9 @@
       <c r="C29" t="s">
         <v>46</v>
       </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
       <c r="F29" s="2" t="s">
         <v>123</v>
       </c>

</xml_diff>

<commit_message>
Fixed plot_logindex and debugged non-parametric sel
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -345,9 +345,6 @@
     <t>sex codes: 0=combined; 1=use female only; 2=use male only; 3 = joint female and male</t>
   </si>
   <si>
-    <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic</t>
-  </si>
-  <si>
     <t>Survey and fishery data specifications</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>Numeric: number of foraging days per year for each species</t>
+  </si>
+  <si>
+    <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic; 5 = non-parametric selectivity sensu Taylor et al 2014 (Hake)</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>30</v>
@@ -1368,13 +1368,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
         <v>85</v>
@@ -1391,13 +1391,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -1414,13 +1414,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
         <v>85</v>
@@ -1437,13 +1437,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
@@ -1460,13 +1460,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
         <v>85</v>
@@ -1475,7 +1475,7 @@
         <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,13 +1483,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" t="s">
         <v>85</v>
@@ -1498,7 +1498,7 @@
         <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1506,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
         <v>85</v>
@@ -1529,13 +1529,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
         <v>85</v>
@@ -1544,7 +1544,7 @@
         <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,13 +1552,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
         <v>85</v>
@@ -1575,13 +1575,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
         <v>85</v>
@@ -1598,13 +1598,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
         <v>85</v>
@@ -1621,13 +1621,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
         <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
         <v>85</v>
@@ -1644,13 +1644,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
         <v>85</v>
@@ -1667,13 +1667,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
         <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1690,22 +1690,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
         <v>85</v>
       </c>
       <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
         <v>127</v>
-      </c>
-      <c r="G16" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1713,13 +1713,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
         <v>85</v>
@@ -1736,13 +1736,13 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
         <v>134</v>
-      </c>
-      <c r="D18" t="s">
-        <v>135</v>
       </c>
       <c r="E18" t="s">
         <v>85</v>
@@ -1751,7 +1751,7 @@
         <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1759,19 +1759,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
         <v>85</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
         <v>58</v>
@@ -1782,13 +1782,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
         <v>85</v>
@@ -1797,7 +1797,7 @@
         <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,13 +1805,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E21" t="s">
         <v>85</v>
@@ -1820,7 +1820,7 @@
         <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1831,13 +1831,13 @@
         <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
         <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
         <v>72</v>
@@ -1888,10 +1888,10 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
         <v>121</v>
-      </c>
-      <c r="D25" t="s">
-        <v>122</v>
       </c>
       <c r="E25" t="s">
         <v>85</v>
@@ -1908,10 +1908,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
         <v>119</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
       <c r="E26" t="s">
         <v>85</v>
@@ -1931,7 +1931,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
         <v>85</v>
@@ -2055,13 +2055,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F35" t="s">
         <v>76</v>
@@ -2072,13 +2072,13 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2086,13 +2086,13 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2101,13 +2101,13 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
         <v>20</v>
@@ -2129,7 +2129,7 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
@@ -2143,7 +2143,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
@@ -2157,7 +2157,7 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -2171,7 +2171,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -2185,7 +2185,7 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -2199,7 +2199,7 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -2213,7 +2213,7 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
         <v>27</v>
@@ -2227,10 +2227,10 @@
         <v>39</v>
       </c>
       <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
         <v>117</v>
-      </c>
-      <c r="D47" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updating vignette for selectivity
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -186,9 +186,6 @@
     <t>Species number</t>
   </si>
   <si>
-    <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2. Not used otherwise</t>
-  </si>
-  <si>
     <t>Units used for survey: 1 = kg; 2 = numbers</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity, or descending logistic. 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
-  </si>
-  <si>
     <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 2 = random effect, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y</t>
   </si>
   <si>
@@ -502,6 +496,12 @@
   </si>
   <si>
     <t>Selectivity to use for the species: 0 = empirical selectivity provided in srv_emp_sel; 1 = logistic selectivity; 2 = non-parametric selecitivty sensu Ianelli et al 2018; 3 = double logistic; 4 = descending logistic; 5 = non-parametric selectivity sensu Taylor et al 2014 (Hake)</t>
+  </si>
+  <si>
+    <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2 &amp; 5. Not used otherwise</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1328,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>30</v>
@@ -1357,7 +1357,7 @@
         <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
@@ -1368,22 +1368,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1391,22 +1391,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,22 +1414,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
         <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,16 +1437,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
         <v>135</v>
       </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
-      </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
         <v>48</v>
@@ -1460,22 +1460,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,22 +1483,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
         <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1506,22 +1506,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1529,22 +1529,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,22 +1552,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,22 +1575,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
         <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1598,22 +1598,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" t="s">
         <v>95</v>
-      </c>
-      <c r="G12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1621,22 +1621,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
         <v>97</v>
-      </c>
-      <c r="G13" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,22 +1644,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
         <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1667,22 +1667,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
         <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,22 +1690,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1713,22 +1713,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
         <v>74</v>
-      </c>
-      <c r="G17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,22 +1736,22 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" t="s">
         <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1759,22 +1759,22 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,22 +1782,22 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,22 +1805,22 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1828,19 +1828,19 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1854,13 +1854,13 @@
         <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1874,13 +1874,13 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1888,19 +1888,19 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1908,19 +1908,19 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1931,16 +1931,16 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" t="s">
         <v>103</v>
-      </c>
-      <c r="G27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,13 +1954,13 @@
         <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
         <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1974,13 +1974,13 @@
         <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" t="s">
         <v>105</v>
-      </c>
-      <c r="G29" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,10 +1994,10 @@
         <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
         <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
         <v>40</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,16 +2055,16 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,13 +2072,13 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2086,13 +2086,13 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2101,13 +2101,13 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C39" t="s">
         <v>20</v>
@@ -2129,7 +2129,7 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
@@ -2143,7 +2143,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
@@ -2157,7 +2157,7 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -2171,7 +2171,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -2185,7 +2185,7 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -2199,7 +2199,7 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -2213,7 +2213,7 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C46" t="s">
         <v>27</v>
@@ -2227,10 +2227,10 @@
         <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated multispecies modes and suitability estimation
Updated kinzey and punt 2009 multispecies modes and likelihoods
-multinomial diet prop fit
-lognromal ration fit
Updated lognormal and gamma suitability
Updated vignette
Still a bug or two need to address
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -15,6 +15,7 @@
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -483,9 +484,6 @@
     <t>Integer: switch to estimate or fix numbers-at-age: 0 = estimate dynamics, 1 = use input numbers-at-age in NbyageFixed, 2 = multiply input numbers-at-age (NbyageFixed) by a single scaling coefficient, 3 = multiply input numbers-at-age (NbyageFixed) by age specific scaling coefficient.</t>
   </si>
   <si>
-    <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979)</t>
-  </si>
-  <si>
     <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
   </si>
   <si>
@@ -502,6 +500,9 @@
   </si>
   <si>
     <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1499,7 @@
         <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1521,7 +1522,7 @@
         <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,7 +1545,7 @@
         <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2061,7 +2062,7 @@
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
         <v>75</v>
@@ -2078,7 +2079,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2092,7 +2093,7 @@
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2107,7 +2108,7 @@
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
remove Mn_LatAge and UobsAge
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -15,12 +15,11 @@
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="157">
   <si>
     <t>nspp</t>
   </si>
@@ -67,9 +66,6 @@
     <t>M1_base</t>
   </si>
   <si>
-    <t>Mn_LatAge</t>
-  </si>
-  <si>
     <t>aLW</t>
   </si>
   <si>
@@ -139,9 +135,6 @@
     <t>Residual natural mortality for each species</t>
   </si>
   <si>
-    <t>Mean length-at-age for each species. Used when estimating time-invariant length-based gamma suitability (suitMode = 1) or time invariant length-based lognormal suitability (suitMode = 4)</t>
-  </si>
-  <si>
     <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
   </si>
   <si>
@@ -154,13 +147,7 @@
     <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
   </si>
   <si>
-    <t>UobsAge</t>
-  </si>
-  <si>
     <t>UobsWtAge</t>
-  </si>
-  <si>
-    <t>Stomach proportion by numbers for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
   </si>
   <si>
     <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
@@ -1326,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,25 +1330,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1369,22 +1356,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1392,22 +1379,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
         <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1415,22 +1402,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1438,22 +1425,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1461,22 +1448,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1484,22 +1471,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
         <v>133</v>
       </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
-      </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1507,22 +1494,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,22 +1517,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1553,22 +1540,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,22 +1563,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1599,22 +1586,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1622,22 +1609,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1645,22 +1632,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,22 +1655,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
         <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1691,22 +1678,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,22 +1701,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1737,22 +1724,22 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1760,22 +1747,22 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1783,22 +1770,22 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1806,22 +1793,22 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1829,19 +1816,19 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1852,16 +1839,16 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1872,16 +1859,16 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1889,19 +1876,19 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1909,19 +1896,19 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1932,16 +1919,16 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1952,16 +1939,16 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
         <v>51</v>
-      </c>
-      <c r="G28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1972,16 +1959,16 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1992,13 +1979,13 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,7 +1996,7 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2020,7 +2007,7 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2031,24 +2018,27 @@
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,16 +2046,16 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2073,13 +2063,13 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2087,13 +2077,13 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -2102,13 +2092,13 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,13 +2106,13 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2130,13 +2120,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,13 +2134,13 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2158,13 +2148,13 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2172,13 +2162,13 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2186,13 +2176,13 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2200,27 +2190,24 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
-        <v>134</v>
-      </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,10 +2215,10 @@
         <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,32 +2226,10 @@
         <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>41</v>
-      </c>
-      <c r="C49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>42</v>
-      </c>
-      <c r="C50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update random selectivity deviate switches
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -342,9 +342,6 @@
     <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
   </si>
   <si>
-    <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 2 = random effect, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y</t>
-  </si>
-  <si>
     <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
   </si>
   <si>
@@ -480,10 +477,13 @@
     <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2 &amp; 5. Not used otherwise</t>
   </si>
   <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
-  </si>
-  <si>
     <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
+  </si>
+  <si>
+    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity. "random_sel" treats random deviates and random walk parameters as random effects.</t>
+  </si>
+  <si>
+    <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
   </si>
 </sst>
 </file>
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1330,7 @@
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
@@ -1350,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
         <v>80</v>
@@ -1373,13 +1373,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>80</v>
@@ -1396,13 +1396,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" t="s">
         <v>80</v>
@@ -1419,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
         <v>80</v>
@@ -1442,13 +1442,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
         <v>80</v>
@@ -1457,7 +1457,7 @@
         <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1465,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
         <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
         <v>80</v>
@@ -1480,7 +1480,7 @@
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1488,13 +1488,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
         <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
         <v>80</v>
@@ -1503,7 +1503,7 @@
         <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1511,13 +1511,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
         <v>80</v>
@@ -1534,13 +1534,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
         <v>80</v>
@@ -1557,13 +1557,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
         <v>80</v>
@@ -1580,13 +1580,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
         <v>80</v>
@@ -1603,13 +1603,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
         <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
         <v>80</v>
@@ -1626,13 +1626,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
         <v>80</v>
@@ -1649,13 +1649,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" t="s">
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
         <v>80</v>
@@ -1672,22 +1672,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" t="s">
         <v>80</v>
       </c>
       <c r="F16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s">
         <v>120</v>
-      </c>
-      <c r="G16" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1695,13 +1695,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
         <v>80</v>
@@ -1718,13 +1718,13 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
         <v>126</v>
-      </c>
-      <c r="D18" t="s">
-        <v>127</v>
       </c>
       <c r="E18" t="s">
         <v>80</v>
@@ -1733,7 +1733,7 @@
         <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1741,13 +1741,13 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" t="s">
         <v>80</v>
@@ -1764,13 +1764,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
         <v>80</v>
@@ -1799,7 +1799,7 @@
         <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1847,10 +1847,10 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
         <v>114</v>
-      </c>
-      <c r="D24" t="s">
-        <v>115</v>
       </c>
       <c r="E24" t="s">
         <v>80</v>
@@ -1867,10 +1867,10 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
         <v>112</v>
-      </c>
-      <c r="D25" t="s">
-        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>80</v>
@@ -1890,7 +1890,7 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
         <v>80</v>
@@ -2006,13 +2006,13 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
@@ -2023,13 +2023,13 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F34" t="s">
         <v>62</v>
@@ -2040,13 +2040,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
         <v>71</v>
@@ -2057,13 +2057,13 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
         <v>19</v>
@@ -2086,7 +2086,7 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
         <v>20</v>
@@ -2100,7 +2100,7 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
@@ -2114,7 +2114,7 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
@@ -2128,7 +2128,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -2142,7 +2142,7 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -2156,7 +2156,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -2170,7 +2170,7 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
         <v>26</v>
@@ -2184,10 +2184,10 @@
         <v>37</v>
       </c>
       <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" t="s">
         <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix random walk estimation and init edit
Keeps mean parameter, but turns off first dev.
Finit now = 0 if initMode != 3
Selectivity normalization turned on for Age_max_selected
- if negative, normalizes by max
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96251511-3738-954F-96A4-1F55F65F221A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4630FE8B-3C65-534F-A794-743F0BED64D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35760" yWindow="2340" windowWidth="31540" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="155">
   <si>
     <t>nspp</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>catch_data</t>
+  </si>
+  <si>
+    <t>Age_max_selected</t>
+  </si>
+  <si>
+    <t>Age at which selectivity = 1. If NA, it will not normalize selectivity. If &lt; 0, will normalize selectivity by the max.</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1308,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,10 +1590,10 @@
         <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1606,11 +1612,11 @@
       <c r="E13" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>54</v>
+      <c r="F13" t="s">
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1629,11 +1635,11 @@
       <c r="E14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" t="s">
-        <v>46</v>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1653,10 +1659,10 @@
         <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1676,10 +1682,10 @@
         <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1699,10 +1705,10 @@
         <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1721,11 +1727,11 @@
       <c r="E18" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>96</v>
+      <c r="F18" t="s">
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1744,11 +1750,11 @@
       <c r="E19" t="s">
         <v>76</v>
       </c>
-      <c r="F19" t="s">
-        <v>62</v>
+      <c r="F19" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1768,10 +1774,10 @@
         <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1788,10 +1794,10 @@
         <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1807,11 +1813,11 @@
       <c r="E22" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>87</v>
+      <c r="F22" t="s">
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1828,10 +1834,10 @@
         <v>76</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1848,10 +1854,10 @@
         <v>76</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1868,10 +1874,10 @@
         <v>76</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1888,10 +1894,10 @@
         <v>76</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1907,11 +1913,11 @@
       <c r="E27" t="s">
         <v>76</v>
       </c>
-      <c r="F27" t="s">
-        <v>45</v>
+      <c r="F27" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1927,11 +1933,11 @@
       <c r="E28" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>92</v>
+      <c r="F28" t="s">
+        <v>45</v>
       </c>
       <c r="G28" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1947,6 +1953,12 @@
       <c r="E29" t="s">
         <v>76</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1958,11 +1970,8 @@
       <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" t="s">
-        <v>94</v>
+      <c r="E30" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1974,6 +1983,12 @@
       </c>
       <c r="D31" t="s">
         <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Upper age_max_selected for normalizing across range of ages
Switch checks as well
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\Rceattle\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88D93E-E48A-4C47-950E-A281CB2CA96D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BD06EC-C598-4F3D-9E6F-C40129725B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="765" windowWidth="34560" windowHeight="21585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
   <si>
     <t>nspp</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Sheet name</t>
+  </si>
+  <si>
+    <t>Age_max_selected_upper</t>
+  </si>
+  <si>
+    <t>Upper age for selectivity normalization (default = NA). If NA, does not use the age range, If not NA, uses mean selectivity between `Age_max_selected` and `Age_max_selected_upper`</t>
   </si>
 </sst>
 </file>
@@ -1330,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,39 +1666,40 @@
       <c r="C28" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1700,10 +1707,10 @@
         <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,234 +1718,234 @@
         <v>56</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="6" t="s">
+    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="8" t="s">
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="8" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="8" t="s">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="8" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="8" t="s">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>97</v>
+        <v>56</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" t="s">
-        <v>92</v>
+        <v>10</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,10 +1953,10 @@
         <v>82</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,10 +1964,10 @@
         <v>82</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1968,10 +1975,10 @@
         <v>82</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1979,10 +1986,10 @@
         <v>82</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +1997,10 @@
         <v>82</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2001,7 +2008,7 @@
         <v>82</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
         <v>29</v>
@@ -2012,7 +2019,7 @@
         <v>82</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>29</v>
@@ -2023,7 +2030,7 @@
         <v>82</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -2034,7 +2041,7 @@
         <v>82</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C66" t="s">
         <v>29</v>
@@ -2045,7 +2052,7 @@
         <v>82</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
         <v>29</v>
@@ -2053,48 +2060,59 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+    <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding weighted-mean diet data and documentation
Added weighted mean diet proportion of prey-spp in predator-spp (sum across prey ages and take weighted mean across predator ages)

Added documentation to meta_data about diet data options

Diet_data can now be predicted but not included in likelihood
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\Rceattle\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BD06EC-C598-4F3D-9E6F-C40129725B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189E839-E1F0-4A38-84B5-E0BF69DEF48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="765" windowWidth="34560" windowHeight="21585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="145">
   <si>
     <t>nspp</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
-  </si>
-  <si>
-    <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
   </si>
   <si>
     <t>Species</t>
@@ -461,9 +458,6 @@
 After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
   </si>
   <si>
-    <t>Survey index or fishery indices in weight (kg) or numbers</t>
-  </si>
-  <si>
     <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. 
 Can have multiple matrices for a species specified by Age_transition_index.</t>
   </si>
@@ -498,6 +492,24 @@
   </si>
   <si>
     <t>Upper age for selectivity normalization (default = NA). If NA, does not use the age range, If not NA, uses mean selectivity between `Age_max_selected` and `Age_max_selected_upper`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey index or fishery indices in weight (kg) or numbers. </t>
+  </si>
+  <si>
+    <t>NOTE: For catch, index, and comp data, if "Year" is negative, it will predict for that year, but not include the data in the likelihood.</t>
+  </si>
+  <si>
+    <t>NOTE: For emp_sel, weight, and ration_data, if "Year" == 0, those data will be used for all years</t>
+  </si>
+  <si>
+    <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Multiple diet-data formats can be included:
+1) If Pred_age &gt;= 0 and Prey_age &gt;= 0, data is assumed to be  diet proportion of prey-at-age/sex in predator-at-age/sex. 
+2) If Pred_age &gt;= 0 and Prey_age &lt; 0, data is assumed to be mean diet proportion of prey-spp in predator-at-age/sex (sum across prey ages and sexes)
+3) If Pred_age &lt; 0 and Prey_age &lt; 0, data is assumed to be  mean diet proportion of prey-spp in predator-spp (sum across prey ages/sexes and take mean across predator ages/sexes)
+4) If Pred_age &lt; -500 and Prey_age &lt; 0, data is assumed to be weighted mean diet proportion of prey-spp in predator-spp (sum across prey ages/sexes and take weighted mean across predator ages/sexes). Weights are estimated predators-at-age.
+If "Year = 0", the the diet will be assumed to be the average between "suit_styr" and "suit_endyr". 
+Only diet-data type 1 can be used for MSVPA based suitability</t>
   </si>
 </sst>
 </file>
@@ -1336,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,10 +1365,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -1367,507 +1379,507 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
         <v>46</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" t="s">
         <v>127</v>
-      </c>
-      <c r="C41" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
         <v>66</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
         <v>22</v>
@@ -1875,18 +1887,18 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
         <v>75</v>
-      </c>
-      <c r="C48" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
         <v>73</v>
-      </c>
-      <c r="C49" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1894,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1907,15 +1919,15 @@
     </row>
     <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
         <v>24</v>
@@ -1923,7 +1935,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
@@ -1939,51 +1951,51 @@
     </row>
     <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>13</v>
@@ -1994,7 +2006,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>14</v>
@@ -2005,7 +2017,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>15</v>
@@ -2016,7 +2028,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>16</v>
@@ -2027,7 +2039,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>17</v>
@@ -2038,7 +2050,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>18</v>
@@ -2049,7 +2061,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>19</v>
@@ -2060,7 +2072,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>20</v>
@@ -2071,49 +2083,59 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" t="s">
-        <v>30</v>
+        <v>102</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CAAL updates - compiles and tests w/o CAAL data work
Refactor: Rename Pyrs to "ration_data", old name will still be read in, but name will be updated

Feature: Added internal growth calculation, see \code{build_growth} within \code{fit_mod} wrapper and growth.hpp. Added `beta_wt_len` and `alpha_wt_len` to "control" sheet of data. Added CAAL_loglike and CAAL_weights to fleet control. Added CAAL_data to data.

Feature: Added size based selectivity.

Feature: Added month to "fleet_control"

Refactor: Change Nselages to N_sel_bins

Refactor: renamed N_sel_bins = Nselages, Sel_norm_bin1 = Age_max_selected, and Sel_norm_bin2 = Age_max_selected_upper
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\Rceattle\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189E839-E1F0-4A38-84B5-E0BF69DEF48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6940EDAC-9B17-BB4F-88DF-FDDECB12F63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="34560" windowHeight="21585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="151">
   <si>
     <t>nspp</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Selectivity</t>
   </si>
   <si>
-    <t>Nselages</t>
-  </si>
-  <si>
     <t>Weight_index</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>Age_first_selected</t>
   </si>
   <si>
-    <t>Age at which selectivity is non-zero</t>
-  </si>
-  <si>
     <t>Estimate_catch_sd</t>
   </si>
   <si>
@@ -304,9 +298,6 @@
     <t>Numeric: number of foraging days per year for each species</t>
   </si>
   <si>
-    <t>Number of ages to estimate non-parametric selectivity for Selectivity = 2 &amp; 5. Not used otherwise</t>
-  </si>
-  <si>
     <t>Comp_loglike</t>
   </si>
   <si>
@@ -316,9 +307,6 @@
     <t>catch_data</t>
   </si>
   <si>
-    <t>Age_max_selected</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -350,9 +338,6 @@
   </si>
   <si>
     <t>Index of survey/fishery (does not restart for each species)</t>
-  </si>
-  <si>
-    <t>Index to match selectivities (otherwise, same as fleet_code)</t>
   </si>
   <si>
     <t>Integer: switch to estimate or fix numbers-at-age: 
@@ -388,11 +373,6 @@
 If selectivity is set to type = 2 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
   </si>
   <si>
-    <t>Age at which selectivity = 1. 
-If NA, it will not normalize selectivity. 
-If &lt; 0, will normalize selectivity by the max.</t>
-  </si>
-  <si>
     <t>Composition data distribution:
 -1 = AFSC multinomial
 0 = full multinomial
@@ -466,13 +446,6 @@
 Can have multiple weight-at-age data-sets for each species.</t>
   </si>
   <si>
-    <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 
-1 = Exponential (Stewart et al 1983)
-2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015)
-3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979)
-4 = for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
-  </si>
-  <si>
     <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5 or 6. Will use the mean for missing years. Temperature should be in celcius.</t>
   </si>
   <si>
@@ -486,12 +459,6 @@
   </si>
   <si>
     <t>Sheet name</t>
-  </si>
-  <si>
-    <t>Age_max_selected_upper</t>
-  </si>
-  <si>
-    <t>Upper age for selectivity normalization (default = NA). If NA, does not use the age range, If not NA, uses mean selectivity between `Age_max_selected` and `Age_max_selected_upper`</t>
   </si>
   <si>
     <t xml:space="preserve">Survey index or fishery indices in weight (kg) or numbers. </t>
@@ -510,6 +477,57 @@
 4) If Pred_age &lt; -500 and Prey_age &lt; 0, data is assumed to be weighted mean diet proportion of prey-spp in predator-spp (sum across prey ages/sexes and take weighted mean across predator ages/sexes). Weights are estimated predators-at-age.
 If "Year = 0", the the diet will be assumed to be the average between "suit_styr" and "suit_endyr". 
 Only diet-data type 1 can be used for MSVPA based suitability</t>
+  </si>
+  <si>
+    <t>alpha_wt_len</t>
+  </si>
+  <si>
+    <t>beta_wt_len</t>
+  </si>
+  <si>
+    <t>Alpha parameter from Weight = alpha * Length ^ beta</t>
+  </si>
+  <si>
+    <t>Beta parameter from Weight = alpha * Length ^ beta</t>
+  </si>
+  <si>
+    <t>Index to mirror selectivities (otherwise, same as fleet_code)</t>
+  </si>
+  <si>
+    <t>N_sel_bins</t>
+  </si>
+  <si>
+    <t>Number of age or length bins to estimate non-parametric selectivity for Selectivity = 2 &amp; 5. Not used otherwise</t>
+  </si>
+  <si>
+    <t>Sel_norm_bin1</t>
+  </si>
+  <si>
+    <t>Sel_norm_bin2</t>
+  </si>
+  <si>
+    <t>Upper age/length bin for selectivity normalization (default = NA). If NA, does not use the age range, If not NA, uses mean selectivity between `Age_max_selected` and `Age_max_selected_upper`</t>
+  </si>
+  <si>
+    <t>Age/length bin at which selectivity = 1. 
+If NA, it will not normalize selectivity. 
+If &lt; 0, will normalize selectivity by the max.</t>
+  </si>
+  <si>
+    <t>Age at which selectivity becomes non-zero</t>
+  </si>
+  <si>
+    <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 
+1 = Exponential (Stewart et al 1983)
+2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015)
+3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979)
+4 = for direct input of consumption in Pyrs  where consumption at age = Numbers * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
+  </si>
+  <si>
+    <t>caal_data</t>
+  </si>
+  <si>
+    <t>Survey/fishery CAAL data. Note if sex is 3, put female CAAL data then male CAAL data (similar to SS).</t>
   </si>
 </sst>
 </file>
@@ -1348,27 +1366,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="119.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="119.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -1377,765 +1395,795 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="6" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="6" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C64" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B62" s="6" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C65" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B63" s="6" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C63" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>143</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made sure size-selex works and added
refactor: changed Age_first_selected to Bin_first_selected
refactor: sel to sel_at_age
fix: small bugs
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6940EDAC-9B17-BB4F-88DF-FDDECB12F63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD74161-B810-414B-A58B-4F9D3E63D020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="155">
   <si>
     <t>nspp</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Fleet_type</t>
-  </si>
-  <si>
-    <t>Age_first_selected</t>
   </si>
   <si>
     <t>Estimate_catch_sd</t>
@@ -350,27 +347,6 @@
     <t>0 = Do not estimate (fixes all parameters for this fleet to initial values)
 1 = Fishery
 2 = Survey</t>
-  </si>
-  <si>
-    <t>0 = empirical selectivity provided in srv_emp_sel
-1 = logistic selectivity
-2 = non-parametric selecitivty sensu Ianelli et al 2018
-3 = double logistic
-4 = descending logistic
-5 = non-parametric selectivity sensu Taylor et al 2014 (Hake)</t>
-  </si>
-  <si>
-    <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 
-0 = no
-1 = penalized deviates given sel_sd_prior (or random effects if "random_sel" is selected in "fit_mod"), 
-3 = time blocks with no penality 
-4 = random walk following Dorn
-5 = random walk on ascending portion of double logistic only. 
-If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
-  </si>
-  <si>
-    <t>The sd to use for the random walk of time varying selectivity if set to 1. 
-If selectivity is set to type = 2 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
   </si>
   <si>
     <t>Composition data distribution:
@@ -514,9 +490,6 @@
 If &lt; 0, will normalize selectivity by the max.</t>
   </si>
   <si>
-    <t>Age at which selectivity becomes non-zero</t>
-  </si>
-  <si>
     <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 
 1 = Exponential (Stewart et al 1983)
 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015)
@@ -528,6 +501,48 @@
   </si>
   <si>
     <t>Survey/fishery CAAL data. Note if sex is 3, put female CAAL data then male CAAL data (similar to SS).</t>
+  </si>
+  <si>
+    <t>Bin_first_selected</t>
+  </si>
+  <si>
+    <t>Age/length bin at which selectivity becomes non-zero</t>
+  </si>
+  <si>
+    <t>0 = empirical selectivity provided in srv_emp_sel
+1 = Age-based logistic selectivity
+2 = Age-based non-parametric selecitivty sensu Ianelli et al 2018
+3 = Age-based double logistic
+4 = Age-based descending logistic
+5 = Age-based non-parametric selectivity sensu Taylor et al 2014 (Hake)
+6 = Length-based logistic selectivity
+7 = Length-based non-parametric selecitivty sensu Ianelli et al 2018
+8 = Length-based double logistic
+9 = Length-based descending logistic
+10 = Length-based non-parametric selectivity sensu Taylor et al 2014 (Hake)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 
+0 = no
+1 = penalized deviates given sel_sd_prior (or random effects if "random_sel" is selected in "fit_mod"), 
+3 = time blocks with no penality 
+4 = random walk following Dorn
+5 = random walk on ascending portion of double logistic only. </t>
+  </si>
+  <si>
+    <t>Sel_curve_pen1</t>
+  </si>
+  <si>
+    <t>Sel_curve_pen2</t>
+  </si>
+  <si>
+    <t>The sd to use for the random walk of time varying selectivity if set to 1, 4, or 5.</t>
+  </si>
+  <si>
+    <t>If selectivity is set to type = 2 or 7 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>If selectivity is set to type = 2 or 7 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1383,10 +1398,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -1397,190 +1412,190 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1589,7 +1604,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1611,7 +1626,7 @@
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1623,7 +1638,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1645,10 +1660,10 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>54</v>
       </c>
@@ -1656,7 +1671,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -1665,81 +1680,82 @@
         <v>54</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="E32" s="2"/>
     </row>
@@ -1747,33 +1763,34 @@
       <c r="A33" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" t="s">
-        <v>114</v>
+      <c r="C35" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1781,88 +1798,88 @@
         <v>54</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>115</v>
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>66</v>
+      <c r="B38" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>119</v>
+      <c r="B42" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>120</v>
+      <c r="B43" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1870,10 +1887,10 @@
         <v>54</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1881,21 +1898,21 @@
         <v>54</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1903,194 +1920,194 @@
         <v>54</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s">
-        <v>132</v>
+        <v>54</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>126</v>
+        <v>144</v>
+      </c>
+      <c r="C53" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" t="s">
-        <v>25</v>
+        <v>94</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="6" t="s">
+    <row r="62" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" t="s">
-        <v>90</v>
+      <c r="C62" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C68" t="s">
         <v>29</v>
@@ -2098,10 +2115,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
         <v>29</v>
@@ -2109,10 +2126,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C70" t="s">
         <v>29</v>
@@ -2120,10 +2137,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C71" t="s">
         <v>29</v>
@@ -2131,59 +2148,81 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>99</v>
+        <v>78</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B77" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>38</v>
+      <c r="B79" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>133</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>134</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests, examples, and renames
rename "Catchability" to "Catchability"
rename: "Time_varying_sel_sd_prior" to "Time_varying_sel_sd_prior"
feature: added CAAL data simulation to sim_mod
feature: added CAAL data update run_mse
fix: added check of column names for sex_ratio and maturity to deal with contains("Age") for selecting the columns
Double checked tests and examples to make sure things are running
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_data_names.xlsx
+++ b/inst/extdata/meta_data_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/Rceattle/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD74161-B810-414B-A58B-4F9D3E63D020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0A6E23-7146-7249-BECD-2D0D2B1F9B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="159">
   <si>
     <t>nspp</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Weight_index</t>
   </si>
   <si>
-    <t>Estimate_q</t>
-  </si>
-  <si>
     <t>Species number</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
   </si>
   <si>
     <t>Time_varying_sel</t>
-  </si>
-  <si>
-    <t>Sel_sd_prior</t>
   </si>
   <si>
     <t>Time_varying_q</t>
@@ -536,13 +530,33 @@
     <t>Sel_curve_pen2</t>
   </si>
   <si>
-    <t>The sd to use for the random walk of time varying selectivity if set to 1, 4, or 5.</t>
-  </si>
-  <si>
     <t>If selectivity is set to type = 2 or 7 (non-parametric) this value will be the 1st penalty on selectivity.</t>
   </si>
   <si>
     <t>If selectivity is set to type = 2 or 7 (non-parametric) this value will be the 2nd penalty on selectivity.</t>
+  </si>
+  <si>
+    <t>The fixed or initial sd to use for time varying selectivity if set to 1, 4, or 5.</t>
+  </si>
+  <si>
+    <t>Time_varying_sel_sd_prior</t>
+  </si>
+  <si>
+    <t>Catchability</t>
+  </si>
+  <si>
+    <t>CAAL_loglike</t>
+  </si>
+  <si>
+    <t>CAAL_weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composition weights for CAAL  likelihood. </t>
+  </si>
+  <si>
+    <t>Composition data distribution:
+0 = full multinomial
+1 = dirichlet-multinomial</t>
   </si>
 </sst>
 </file>
@@ -1381,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1398,10 +1412,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -1412,323 +1426,323 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" t="s">
         <v>132</v>
-      </c>
-      <c r="C17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" t="s">
         <v>133</v>
-      </c>
-      <c r="C18" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" t="s">
         <v>150</v>
-      </c>
-      <c r="C27" t="s">
-        <v>153</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" t="s">
         <v>151</v>
-      </c>
-      <c r="C28" t="s">
-        <v>154</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>152</v>
@@ -1737,247 +1751,255 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>105</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>37</v>
+        <v>52</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>111</v>
+      <c r="C39" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>109</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="8" t="s">
+      <c r="C48" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="8" t="s">
+    </row>
+    <row r="49" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C45" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>92</v>
+        <v>52</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>93</v>
+        <v>52</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,148 +2010,142 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>122</v>
+        <v>142</v>
+      </c>
+      <c r="C55" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" t="s">
-        <v>25</v>
+        <v>92</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="6" t="s">
+    <row r="64" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" t="s">
-        <v>89</v>
+      <c r="C64" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
         <v>29</v>
@@ -2137,10 +2153,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C71" t="s">
         <v>29</v>
@@ -2148,10 +2164,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C72" t="s">
         <v>29</v>
@@ -2159,10 +2175,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -2170,59 +2186,81 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>98</v>
+        <v>76</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="C76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>130</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>